<commit_message>
Building the process - Part Two
</commit_message>
<xml_diff>
--- a/Excel reports consolidation/Daily Reports/Coffee Shop 1.xlsx
+++ b/Excel reports consolidation/Daily Reports/Coffee Shop 1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\calin.grigorescu\Documents\UiPath\ExcelConsolidation\Daily Reports\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6c12b539f5863eb1/Documentos/UiPath/Automation-Developer-Professional-Training/Excel reports consolidation/Daily Reports/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FC74FF8-4556-428A-9309-0E051F8DAF42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{3FC74FF8-4556-428A-9309-0E051F8DAF42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BCA9FF79-618E-4C3D-9408-1304483A7851}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3555" yWindow="1965" windowWidth="28800" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>

</xml_diff>

<commit_message>
Publishing and running the process
</commit_message>
<xml_diff>
--- a/Excel reports consolidation/Daily Reports/Coffee Shop 1.xlsx
+++ b/Excel reports consolidation/Daily Reports/Coffee Shop 1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6c12b539f5863eb1/Documentos/UiPath/Automation-Developer-Professional-Training/Excel reports consolidation/Daily Reports/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{3FC74FF8-4556-428A-9309-0E051F8DAF42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BCA9FF79-618E-4C3D-9408-1304483A7851}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{3FC74FF8-4556-428A-9309-0E051F8DAF42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DEA92A4A-051F-4FCF-AAB9-070A7E3FEE8B}"/>
   <bookViews>
-    <workbookView xWindow="3555" yWindow="1965" windowWidth="28800" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8640" yWindow="1875" windowWidth="28800" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -145,6 +145,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>